<commit_message>
added rest of code, and updated planner
</commit_message>
<xml_diff>
--- a/SoftwareEnginneringPlanner.xlsx
+++ b/SoftwareEnginneringPlanner.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bart\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barto\Desktop\corriander\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43ACEF4A-CDE1-4BFA-912F-581A74094C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A628CC9-221D-4751-BC03-EF6801FF02D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="4100" windowWidth="14970" windowHeight="15230" xr2:uid="{A8DAF742-047D-4D73-A30D-622B8B33F8E4}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16903" xr2:uid="{A8DAF742-047D-4D73-A30D-622B8B33F8E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -607,23 +607,23 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8:G9"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="2"/>
-    <col min="2" max="2" width="29.1796875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.90625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.90625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.6328125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.26953125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="8.69140625" style="2"/>
+    <col min="2" max="2" width="29.15234375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.921875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.69140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.921875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.84375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.61328125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.23046875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.69140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="29.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -649,7 +649,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
@@ -675,7 +675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -701,7 +701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -727,7 +727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
@@ -744,7 +744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
@@ -778,7 +778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -798,13 +798,13 @@
         <v>31</v>
       </c>
       <c r="G8" s="4">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="H8" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -828,7 +828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -854,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -880,11 +880,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="5.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -901,7 +901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>32</v>
       </c>
@@ -918,7 +918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -935,7 +935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -952,7 +952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -969,7 +969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
@@ -986,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
@@ -1003,11 +1003,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>32</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
@@ -1205,12 +1205,12 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="13.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1242,12 +1242,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
updated planner, started implemented newly learnt data structures.
</commit_message>
<xml_diff>
--- a/SoftwareEnginneringPlanner.xlsx
+++ b/SoftwareEnginneringPlanner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barto\Desktop\corriander\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A628CC9-221D-4751-BC03-EF6801FF02D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35296FF7-5262-4A52-B758-369C82286FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="25920" windowHeight="16903" xr2:uid="{A8DAF742-047D-4D73-A30D-622B8B33F8E4}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="39">
   <si>
     <t>Topic</t>
   </si>
@@ -607,7 +607,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -737,7 +737,16 @@
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="3">
+      <c r="D5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="4">
         <v>0</v>
       </c>
       <c r="H5" s="3">
@@ -754,9 +763,16 @@
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="3">
         <v>0</v>
       </c>
@@ -771,9 +787,16 @@
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="4"/>
       <c r="H7" s="3">
         <v>0</v>
       </c>
@@ -1102,10 +1125,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G5:G7"/>
   </mergeCells>
-  <conditionalFormatting sqref="G1:H2 G4:H8 G10:H1048576 H9">
+  <conditionalFormatting sqref="G1:H2 G4:H5 G10:H1048576 H9 G8:H8 H6:H7">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1117,7 +1141,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H2 G4:H8 G10:H25 H9">
+  <conditionalFormatting sqref="G2:H2 G4:H5 G10:H25 H9 G8:H8 H6:H7">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -1172,7 +1196,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{572AEE92-4952-4DE8-AB17-D2D7DB409BC2}">
           <x14:formula1>
             <xm:f>Sheet2!$B$2:$B$4</xm:f>

</xml_diff>

<commit_message>
updated settings and planner
</commit_message>
<xml_diff>
--- a/SoftwareEnginneringPlanner.xlsx
+++ b/SoftwareEnginneringPlanner.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barto\Desktop\corriander\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\corriander\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB984BF-8FE4-4063-9829-6D90D37B034F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF503137-D7BE-46E8-A8C5-1F84303CD6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3394" yWindow="3394" windowWidth="19286" windowHeight="12232" xr2:uid="{A8DAF742-047D-4D73-A30D-622B8B33F8E4}"/>
+    <workbookView xWindow="9940" yWindow="3410" windowWidth="14970" windowHeight="15230" xr2:uid="{A8DAF742-047D-4D73-A30D-622B8B33F8E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -607,23 +607,23 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.69140625" style="2"/>
-    <col min="2" max="2" width="29.15234375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.921875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.69140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.921875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.84375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.61328125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.23046875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.69140625" style="2"/>
+    <col min="1" max="1" width="8.7265625" style="2"/>
+    <col min="2" max="2" width="29.1796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.90625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.6328125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="29.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -649,7 +649,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
@@ -675,7 +675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -701,7 +701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -727,7 +727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
@@ -741,19 +741,19 @@
         <v>31</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G5" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H5" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -764,10 +764,10 @@
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>38</v>
@@ -777,7 +777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
@@ -791,7 +791,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>38</v>
@@ -801,7 +801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -827,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -851,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -877,7 +877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -903,11 +903,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="5.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -924,7 +924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>32</v>
       </c>
@@ -941,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -958,7 +958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -975,7 +975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -992,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
@@ -1026,11 +1026,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>32</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D26" s="2">
         <v>1</v>
       </c>
@@ -1234,12 +1234,12 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.07421875" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1271,12 +1271,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
updated planner +1 questions done.
</commit_message>
<xml_diff>
--- a/SoftwareEnginneringPlanner.xlsx
+++ b/SoftwareEnginneringPlanner.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\corriander\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barto\Desktop\corriander\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF503137-D7BE-46E8-A8C5-1F84303CD6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17605867-0DD6-46F6-B84F-C52B182FAF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9940" yWindow="3410" windowWidth="14970" windowHeight="15230" xr2:uid="{A8DAF742-047D-4D73-A30D-622B8B33F8E4}"/>
+    <workbookView xWindow="3394" yWindow="3394" windowWidth="19286" windowHeight="12232" xr2:uid="{A8DAF742-047D-4D73-A30D-622B8B33F8E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -607,23 +607,23 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5:G7"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="2"/>
-    <col min="2" max="2" width="29.1796875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.90625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.90625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.6328125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.26953125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="8.69140625" style="2"/>
+    <col min="2" max="2" width="29.15234375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.921875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.69140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.921875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.84375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.61328125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.23046875" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.69140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="29.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -649,7 +649,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
@@ -675,7 +675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -701,7 +701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -727,7 +727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
@@ -747,13 +747,13 @@
         <v>31</v>
       </c>
       <c r="G5" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H5" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -777,7 +777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
@@ -801,7 +801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>30</v>
       </c>
@@ -827,7 +827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -851,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -877,7 +877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -903,11 +903,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="5.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>32</v>
       </c>
@@ -924,7 +924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
         <v>32</v>
       </c>
@@ -941,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -958,7 +958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -975,7 +975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -992,7 +992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
@@ -1026,11 +1026,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>32</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>32</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="D26" s="2">
         <v>1</v>
       </c>
@@ -1234,12 +1234,12 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="13.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1271,12 +1271,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Updated planner, Transferred LinkedList into project. Starting Q5 of LinkedLists
</commit_message>
<xml_diff>
--- a/SoftwareEnginneringPlanner.xlsx
+++ b/SoftwareEnginneringPlanner.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barto\Desktop\corriander\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\corriander\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17605867-0DD6-46F6-B84F-C52B182FAF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D01EFF-C215-47B3-9CE5-AF4B044E3D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3394" yWindow="3394" windowWidth="19286" windowHeight="12232" xr2:uid="{A8DAF742-047D-4D73-A30D-622B8B33F8E4}"/>
+    <workbookView xWindow="58230" yWindow="9555" windowWidth="14970" windowHeight="15345" xr2:uid="{A8DAF742-047D-4D73-A30D-622B8B33F8E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -146,9 +146,6 @@
     <t>Own Implemention</t>
   </si>
   <si>
-    <t>Practice Questions</t>
-  </si>
-  <si>
     <t>Review Practice Questions</t>
   </si>
   <si>
@@ -177,6 +174,9 @@
   </si>
   <si>
     <t>Todo</t>
+  </si>
+  <si>
+    <t>Init Practice Questions</t>
   </si>
 </sst>
 </file>
@@ -607,23 +607,23 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8:G9"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.69140625" style="2"/>
-    <col min="2" max="2" width="29.15234375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.921875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.69140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.921875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.84375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.61328125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.23046875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.69140625" style="2"/>
+    <col min="1" max="1" width="8.7265625" style="2"/>
+    <col min="2" max="2" width="29.1796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.90625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.6328125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="29.6" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -643,56 +643,56 @@
         <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2" s="3">
         <v>3</v>
       </c>
       <c r="H2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="3">
         <v>4</v>
@@ -701,24 +701,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -727,24 +727,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="4">
         <v>3</v>
@@ -753,72 +753,72 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" s="4">
         <v>3</v>
@@ -827,48 +827,48 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" s="3">
         <v>0</v>
@@ -877,24 +877,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" s="3">
         <v>0</v>
@@ -903,16 +903,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="5.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>15</v>
@@ -924,12 +924,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>16</v>
@@ -941,12 +941,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>17</v>
@@ -958,12 +958,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>18</v>
@@ -975,12 +975,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>19</v>
@@ -992,12 +992,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>20</v>
@@ -1009,12 +1009,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>21</v>
@@ -1026,28 +1026,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G21" s="3">
         <v>5</v>
@@ -1056,12 +1056,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>23</v>
@@ -1073,12 +1073,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>24</v>
@@ -1090,12 +1090,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>25</v>
@@ -1107,12 +1107,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>26</v>
@@ -1124,7 +1124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D26" s="2">
         <v>1</v>
       </c>
@@ -1234,12 +1234,12 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.07421875" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1247,38 +1247,38 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated study planner created practice_1.cs started whiteboard code for q1 updated test code for q1
</commit_message>
<xml_diff>
--- a/SoftwareEnginneringPlanner.xlsx
+++ b/SoftwareEnginneringPlanner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\corriander\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8678A612-E93B-45B8-A9D6-FB3009199B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430AD5FC-1E96-4B94-9394-61270D9362FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6250" yWindow="4280" windowWidth="18220" windowHeight="15350" xr2:uid="{A8DAF742-047D-4D73-A30D-622B8B33F8E4}"/>
   </bookViews>
@@ -607,7 +607,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1124,7 +1124,7 @@
         <v>23</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
planner update, partial flashcards created for Bit manipulation
</commit_message>
<xml_diff>
--- a/SoftwareEnginneringPlanner.xlsx
+++ b/SoftwareEnginneringPlanner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\corriander\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB589625-4CEE-42B3-83B4-B21F5E4D3967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FB897E-E3DE-4F33-8C29-A4B6623DB954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6250" yWindow="4280" windowWidth="18220" windowHeight="15350" xr2:uid="{A8DAF742-047D-4D73-A30D-622B8B33F8E4}"/>
   </bookViews>
@@ -607,7 +607,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -729,7 +729,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>33</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>33</v>
@@ -777,7 +777,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>33</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>33</v>
@@ -825,7 +825,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>33</v>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>34</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>34</v>
@@ -1127,7 +1127,7 @@
         <v>30</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>37</v>
@@ -1332,7 +1332,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A25 D2:F25</xm:sqref>
+          <xm:sqref>D2:F25 A2:A25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>